<commit_message>
change jdocs copy user and address logist
</commit_message>
<xml_diff>
--- a/demo_docs/data_main.xlsx
+++ b/demo_docs/data_main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>立案日期</t>
   </si>
@@ -46,109 +46,64 @@
     <t>add_index</t>
   </si>
   <si>
-    <t>2018-01-12</t>
-  </si>
-  <si>
-    <t>（2018）XX111</t>
-  </si>
-  <si>
-    <t>（2018）AA111</t>
+    <t>2016-11-15</t>
+  </si>
+  <si>
+    <t>（2018）XX112号</t>
+  </si>
+  <si>
+    <t>（2018）AA112号</t>
   </si>
   <si>
     <t>法官1</t>
   </si>
   <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>2016-11-15</t>
-  </si>
-  <si>
-    <t>（2018）XX112</t>
-  </si>
-  <si>
-    <t>（2018）AA112</t>
-  </si>
-  <si>
     <t>申请人:邓XX, 被申请人:何XX</t>
   </si>
   <si>
-    <t>邓XX/地址：XXXX市XXXXA，何XX/地址：</t>
-  </si>
-  <si>
-    <t>（2018）XX113</t>
-  </si>
-  <si>
-    <t>（2018）AA113</t>
-  </si>
-  <si>
-    <t>申请人:罗XX, 被申请人:樊XX, 原审被告:罗XX（又名罗AA）</t>
+    <t>邓XX_123123213</t>
+  </si>
+  <si>
+    <t>邓XX/地址：广东省佛山市顺德区，何XX/地址：广东省佛山市顺德区</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>（2018）XX113号</t>
+  </si>
+  <si>
+    <t>（2018）AA113号</t>
+  </si>
+  <si>
+    <t>申请人:罗XX, 被申请人:樊XX, 原审被告:罗XX（又名罗aa）</t>
   </si>
   <si>
     <t>2017-07-12</t>
   </si>
   <si>
-    <t>（2018）XX114</t>
-  </si>
-  <si>
-    <t>（2018）AA114</t>
+    <t>（2018）XX114号</t>
+  </si>
+  <si>
+    <t>（2018）AA114号</t>
   </si>
   <si>
     <t>法官2</t>
   </si>
   <si>
-    <t>申请人:莫XX, 被申请人:林XX、张XX</t>
-  </si>
-  <si>
-    <t>2017-09-12</t>
-  </si>
-  <si>
-    <t>（2018）XX115</t>
-  </si>
-  <si>
-    <t>（2018）AA115</t>
-  </si>
-  <si>
-    <t>（2018）XX111号</t>
-  </si>
-  <si>
-    <t>（2018）AA111号</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>（2018）XX112号</t>
-  </si>
-  <si>
-    <t>（2018）AA112号</t>
-  </si>
-  <si>
-    <t>申请人:邓XX, 被申请人:XXX</t>
-  </si>
-  <si>
-    <t>（2018）XX113号</t>
-  </si>
-  <si>
-    <t>（2018）AA113号</t>
-  </si>
-  <si>
-    <t>申请人:罗XX, 被申请人:樊XX, 原审被告:罗XX（又名罗aa）</t>
-  </si>
-  <si>
-    <t>（2018）XX114号</t>
-  </si>
-  <si>
-    <t>（2018）AA114号</t>
-  </si>
-  <si>
     <t>申请人:莫XX, 被申请人:林XX、何XX</t>
   </si>
   <si>
-    <t>（2018）XX115号</t>
-  </si>
-  <si>
-    <t>（2018）AA115号</t>
+    <t>（2018）XX1111号</t>
+  </si>
+  <si>
+    <t>（2018）AA2222号</t>
+  </si>
+  <si>
+    <t>邓XX/傻子_123123123</t>
+  </si>
+  <si>
+    <t>傻子/地址：广东省佛是的，何XX/地址：广东省佛山市顺德区</t>
   </si>
 </sst>
 </file>
@@ -237,22 +192,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
     <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1" vertical="center"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="0"/>
     </xf>
   </cellXfs>
@@ -553,7 +504,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,8 +513,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="18"/>
-    <col customWidth="1" max="2" min="2" width="20.4"/>
-    <col customWidth="1" max="3" min="3" width="20.4"/>
+    <col customWidth="1" max="2" min="2" width="21.6"/>
+    <col customWidth="1" max="3" min="3" width="21.6"/>
     <col customWidth="1" max="4" min="4" width="9.6"/>
     <col customWidth="1" max="5" min="5" width="60"/>
     <col customWidth="1" max="6" min="6" width="60"/>
@@ -618,225 +569,95 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s"/>
-      <c r="F2" s="3" t="s"/>
-      <c r="G2" s="3" t="s"/>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="H2" s="2" t="s"/>
       <c r="I2" s="2" t="s"/>
       <c r="J2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s"/>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="G3" s="3" t="s"/>
       <c r="H3" s="2" t="s"/>
       <c r="I3" s="2" t="s"/>
       <c r="J3" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s"/>
       <c r="G4" s="3" t="s"/>
       <c r="H4" s="2" t="s"/>
       <c r="I4" s="2" t="s"/>
       <c r="J4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s"/>
-      <c r="G5" s="3" t="s"/>
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H5" s="2" t="s"/>
       <c r="I5" s="2" t="s"/>
       <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="3" t="s"/>
-      <c r="F6" s="3" t="s"/>
-      <c r="G6" s="3" t="s"/>
-      <c r="H6" s="2" t="s"/>
-      <c r="I6" s="2" t="s"/>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s"/>
-      <c r="F7" s="3" t="s"/>
-      <c r="G7" s="3" t="s"/>
-      <c r="H7" s="4" t="s"/>
-      <c r="I7" s="4" t="s"/>
-      <c r="J7" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="3" t="s"/>
-      <c r="G8" s="3" t="s"/>
-      <c r="H8" s="4" t="s"/>
-      <c r="I8" s="4" t="s"/>
-      <c r="J8" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="3" t="s"/>
-      <c r="G9" s="3" t="s"/>
-      <c r="H9" s="4" t="s"/>
-      <c r="I9" s="4" t="s"/>
-      <c r="J9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="3" t="s"/>
-      <c r="G10" s="3" t="s"/>
-      <c r="H10" s="4" t="s"/>
-      <c r="I10" s="4" t="s"/>
-      <c r="J10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="3" t="s"/>
-      <c r="F11" s="3" t="s"/>
-      <c r="G11" s="3" t="s"/>
-      <c r="H11" s="4" t="s"/>
-      <c r="I11" s="4" t="s"/>
-      <c r="J11" s="4" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new serise cases func
</commit_message>
<xml_diff>
--- a/demo_docs/data_main.xlsx
+++ b/demo_docs/data_main.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="8250"/>
+    <workbookView windowWidth="17850" windowHeight="7256"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,17 +14,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>立案日期</t>
   </si>
   <si>
+    <t>适用程序</t>
+  </si>
+  <si>
     <t>案号</t>
   </si>
   <si>
     <t>原一审案号</t>
   </si>
   <si>
+    <t>判决书源号</t>
+  </si>
+  <si>
     <t>主审法官</t>
   </si>
   <si>
@@ -37,18 +43,32 @@
     <t>地址</t>
   </si>
   <si>
-    <t>备注1</t>
-  </si>
-  <si>
-    <t>备注2</t>
-  </si>
-  <si>
     <t>add_index</t>
   </si>
   <si>
     <t>2016-11-15</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>BBB_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>集合</t>
+    </r>
+  </si>
+  <si>
     <t>（2018）XX1111号</t>
   </si>
   <si>
@@ -70,6 +90,9 @@
     <t>old</t>
   </si>
   <si>
+    <t>DDD_集合</t>
+  </si>
+  <si>
     <t>（2018）XX112号</t>
   </si>
   <si>
@@ -80,6 +103,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>邓</t>
     </r>
     <r>
@@ -228,13 +257,168 @@
     </r>
   </si>
   <si>
-    <t>（2018）XX113号</t>
-  </si>
-  <si>
-    <t>（2018）AA113号</t>
-  </si>
-  <si>
-    <r>
+    <r>
+      <t>XX113-XX115_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>集合</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>XX113-XX115</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>AA113</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>AA11111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>申请人</t>
     </r>
     <r>
@@ -366,6 +550,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>罗</t>
     </r>
     <r>
@@ -416,6 +606,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>罗</t>
     </r>
     <r>
@@ -462,37 +658,68 @@
     <t>2017-07-12</t>
   </si>
   <si>
-    <t>（2018）XX114号</t>
-  </si>
-  <si>
-    <t>（2018）AA114号</t>
+    <r>
+      <t>AAA_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>集合</t>
+    </r>
+  </si>
+  <si>
+    <t>（2018）XX111号</t>
+  </si>
+  <si>
+    <r>
+      <t>（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2018</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>AA111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>号</t>
+    </r>
   </si>
   <si>
     <t>法官2</t>
   </si>
   <si>
     <t>申请人:莫XX, 被申请人:林XX、何XX</t>
-  </si>
-  <si>
-    <t>2017-09-12</t>
-  </si>
-  <si>
-    <t>（2018）XX115号</t>
-  </si>
-  <si>
-    <t>（2018）AA115号</t>
-  </si>
-  <si>
-    <t>申请人:XXX, 被申请人:XXX</t>
-  </si>
-  <si>
-    <t>2018-01-12</t>
-  </si>
-  <si>
-    <t>（2018）XX111号</t>
-  </si>
-  <si>
-    <t>（2018）AA111号</t>
   </si>
 </sst>
 </file>
@@ -500,12 +727,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,14 +761,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -556,7 +843,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -570,104 +889,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -676,9 +897,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -705,13 +925,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,43 +1021,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,49 +1069,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,55 +1087,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -910,24 +1130,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,9 +1151,59 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -971,218 +1223,219 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="13" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="12" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="51">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
     <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
@@ -1195,43 +1448,45 @@
     <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
     <cellStyle name="超链接" xfId="10" builtinId="8"/>
     <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="-1926604369" xfId="12"/>
+    <cellStyle name="-1363170513" xfId="13"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9"/>
+    <cellStyle name="注释" xfId="15" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="16" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="17" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="18" builtinId="11"/>
+    <cellStyle name="标题" xfId="19" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="20" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="21" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="22" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="23" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="24" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="25" builtinId="44"/>
+    <cellStyle name="输出" xfId="26" builtinId="21"/>
+    <cellStyle name="计算" xfId="27" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="28" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="29" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="30" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="31" builtinId="24"/>
+    <cellStyle name="汇总" xfId="32" builtinId="25"/>
+    <cellStyle name="好" xfId="33" builtinId="26"/>
+    <cellStyle name="适中" xfId="34" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="36" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="37" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="38" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="39" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="40" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="41" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="42" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="43" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="44" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="45" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="46" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="47" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="48" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="49" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="50" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1527,208 +1782,174 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="21.6" customWidth="1"/>
-    <col min="4" max="4" width="9.6" customWidth="1"/>
-    <col min="5" max="7" width="60" customWidth="1"/>
-    <col min="8" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="9.6" customWidth="1"/>
+    <col min="2" max="2" width="20.4017857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7946428571429" customWidth="1"/>
+    <col min="4" max="4" width="21.5982142857143" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5267857142857" customWidth="1"/>
+    <col min="7" max="9" width="60" customWidth="1"/>
+    <col min="10" max="10" width="9.59821428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="30.85" spans="1:10">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:10">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="15.45" spans="1:10">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" ht="15.5" spans="1:10">
-      <c r="A3" s="2" t="s">
+    <row r="3" ht="15.45" spans="1:10">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
+    </row>
+    <row r="4" ht="15.45" spans="1:10">
+      <c r="A4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>17</v>
+      <c r="G4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="4" ht="15.5" spans="1:10">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+    <row r="5" ht="15.45" spans="1:10">
+      <c r="A5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" ht="15.5" spans="1:10">
-      <c r="A5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="F5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" ht="15.5" spans="1:10">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" ht="15.5" spans="1:10">
-      <c r="A7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>